<commit_message>
Added CW_1* which was made by @wojsikora
</commit_message>
<xml_diff>
--- a/CW_11_Modul_Younga/fiz.xlsx
+++ b/CW_11_Modul_Younga/fiz.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Material</t>
   </si>
@@ -61,6 +61,36 @@
   </si>
   <si>
     <t>LINECOS</t>
+  </si>
+  <si>
+    <t>Średnica średnia d [mm]</t>
+  </si>
+  <si>
+    <t>Drut</t>
+  </si>
+  <si>
+    <t>Wartość współczynnika a [mm/N]</t>
+  </si>
+  <si>
+    <t>Wartość współczynnika b [mm/N]</t>
+  </si>
+  <si>
+    <t>u(a)</t>
+  </si>
+  <si>
+    <t>u(b)</t>
+  </si>
+  <si>
+    <t>Wartość współczynnika korelacji y [mm]</t>
+  </si>
+  <si>
+    <t>u(y) [mm]</t>
+  </si>
+  <si>
+    <t>stalowy</t>
+  </si>
+  <si>
+    <t>mosiężny</t>
   </si>
 </sst>
 </file>
@@ -1378,6 +1408,44 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 0,0151</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="pl-PL" baseline="0"/>
+                      <a:t>1</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x + 0,0</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="pl-PL" baseline="0"/>
+                      <a:t>577</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2014,6 +2082,40 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 0,015</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="pl-PL" baseline="0"/>
+                      <a:t>58</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>x + 0,150</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4712,15 +4814,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:colOff>1148080</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>110491</xdr:rowOff>
+      <xdr:rowOff>118956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4741,16 +4843,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1603811</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>75855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622640</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>2445</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4772,15 +4874,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1163238</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>46939</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>741045</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:colOff>116540</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4803,16 +4905,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1712820</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>53787</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>645459</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5099,10 +5201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M88"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71:L75"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5112,9 +5214,12 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="42.77734375" customWidth="1"/>
     <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="19.109375" customWidth="1"/>
     <col min="10" max="10" width="11.109375" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
     <col min="13" max="13" width="37" customWidth="1"/>
     <col min="14" max="14" width="16.21875" customWidth="1"/>
   </cols>
@@ -5175,7 +5280,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0.77</v>
@@ -5819,12 +5924,18 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>13</v>
       </c>
+      <c r="O68">
+        <v>1.55759239727657E-2</v>
+      </c>
+      <c r="P68">
+        <v>0.1508616641283656</v>
+      </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>4.91</v>
       </c>
@@ -5832,13 +5943,19 @@
         <v>0.1075</v>
       </c>
       <c r="D69">
-        <v>1.5105909857590217E-2</v>
+        <v>1.5105909857590199E-2</v>
       </c>
       <c r="E69">
         <v>5.7720112784816098E-2</v>
       </c>
+      <c r="O69">
+        <v>6.8996197183907547E-4</v>
+      </c>
+      <c r="P69">
+        <v>2.4908911033833629E-2</v>
+      </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>9.81</v>
       </c>
@@ -5854,8 +5971,14 @@
       <c r="K70" t="s">
         <v>13</v>
       </c>
+      <c r="O70">
+        <v>0.98075563940381227</v>
+      </c>
+      <c r="P70">
+        <v>4.0469039989071427E-2</v>
+      </c>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>14.72</v>
       </c>
@@ -5878,8 +6001,14 @@
       <c r="M71" t="e">
         <v>#N/A</v>
       </c>
+      <c r="O71">
+        <v>509.63274903407302</v>
+      </c>
+      <c r="P71">
+        <v>10</v>
+      </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>19.62</v>
       </c>
@@ -5901,8 +6030,14 @@
       <c r="M72" t="e">
         <v>#N/A</v>
       </c>
+      <c r="O72">
+        <v>0.83464756802362927</v>
+      </c>
+      <c r="P72">
+        <v>1.6377431976370625E-2</v>
+      </c>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>24.53</v>
       </c>
@@ -5925,7 +6060,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B74">
         <v>29.43</v>
       </c>
@@ -5942,7 +6077,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>34.340000000000003</v>
       </c>
@@ -5959,7 +6094,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>39.24</v>
       </c>
@@ -5976,7 +6111,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>44.15</v>
       </c>
@@ -5993,7 +6128,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B78">
         <v>49.05</v>
       </c>
@@ -6001,7 +6136,7 @@
         <v>0.8175</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B79">
         <v>53.96</v>
       </c>
@@ -6009,15 +6144,19 @@
         <v>0.86749999999999994</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>58.86</v>
       </c>
       <c r="C80">
         <v>0.94750000000000001</v>
       </c>
+      <c r="E80">
+        <f>(4*1.059)/(PI()*(B4*0.001)^2 * (D69*0.001))</f>
+        <v>150548953028.41714</v>
+      </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B81">
         <v>63.77</v>
       </c>
@@ -6025,7 +6164,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B82">
         <v>68.67</v>
       </c>
@@ -6033,15 +6172,19 @@
         <v>1.085</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>73.58</v>
       </c>
       <c r="C83">
         <v>1.175</v>
       </c>
+      <c r="E83">
+        <f>(4*1.063)/(3.14*(0.00183)^2 * 0.00001558)</f>
+        <v>25953382952.993374</v>
+      </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B84">
         <v>78.48</v>
       </c>
@@ -6049,31 +6192,98 @@
         <v>1.2475000000000001</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B85">
         <v>83.39</v>
       </c>
       <c r="C85">
         <v>1.2949999999999999</v>
       </c>
+      <c r="G85" t="s">
+        <v>15</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
+      </c>
+      <c r="I85" t="s">
+        <v>18</v>
+      </c>
+      <c r="J85" t="s">
+        <v>17</v>
+      </c>
+      <c r="K85" t="s">
+        <v>19</v>
+      </c>
+      <c r="L85" t="s">
+        <v>20</v>
+      </c>
+      <c r="M85" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B86">
         <v>88.29</v>
       </c>
       <c r="C86">
         <v>1.375</v>
       </c>
+      <c r="E86">
+        <f>(4*1.063)/(3.14*(0.00183)^2 * 0.00001558)</f>
+        <v>25953382952.993374</v>
+      </c>
+      <c r="G86" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86">
+        <v>1.511E-2</v>
+      </c>
+      <c r="I86">
+        <v>1.1E-4</v>
+      </c>
+      <c r="J86">
+        <v>5.772E-2</v>
+      </c>
+      <c r="K86">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="L86">
+        <v>0.999</v>
+      </c>
+      <c r="M86">
+        <v>1.4E-2</v>
+      </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B87">
         <v>93.2</v>
       </c>
       <c r="C87">
         <v>1.4525000000000001</v>
       </c>
+      <c r="G87" t="s">
+        <v>23</v>
+      </c>
+      <c r="H87">
+        <v>1.558E-2</v>
+      </c>
+      <c r="I87">
+        <v>6.8999999999999997E-4</v>
+      </c>
+      <c r="J87">
+        <v>0.15</v>
+      </c>
+      <c r="K87">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L87">
+        <v>0.98</v>
+      </c>
+      <c r="M87">
+        <v>0.04</v>
+      </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B88">
         <v>98.1</v>
       </c>

</xml_diff>